<commit_message>
add classes for votes and session v5
</commit_message>
<xml_diff>
--- a/design concept/DatenbankExcel.xlsx
+++ b/design concept/DatenbankExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dua\Git\Game2gather\design concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BE7A17-4A1A-4407-BD05-D0848CD82C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A99C68-63BC-420F-86E5-78D19CBE63DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{88A67D36-E61D-4BAE-8D7E-BAA3FC990866}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Session</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Lastname</t>
   </si>
   <si>
-    <t>Enum_Value</t>
-  </si>
-  <si>
     <t>FK_Player_Id</t>
   </si>
   <si>
@@ -143,12 +140,6 @@
     <t>FoodOption</t>
   </si>
   <si>
-    <t>Votevalue</t>
-  </si>
-  <si>
-    <t>FK_Votevalue_Id</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -179,10 +170,10 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Spalte1</t>
-  </si>
-  <si>
     <t>Vote</t>
+  </si>
+  <si>
+    <t>Vote_value</t>
   </si>
 </sst>
 </file>
@@ -236,7 +227,7 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="5">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -248,9 +239,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -278,26 +266,15 @@
     <tableColumn id="4" xr3:uid="{85781AB9-25B7-446D-900C-B11DC2028C7F}" name="DatePlayed"/>
     <tableColumn id="5" xr3:uid="{6C494DDF-E595-4DD7-9DCB-7D3CF5B99AE1}" name="Voting_Link"/>
     <tableColumn id="6" xr3:uid="{88A7D363-E97E-4D81-8A62-116AF6D68C0D}" name="Max_Player"/>
-    <tableColumn id="7" xr3:uid="{5BDF043D-B9D7-4535-B485-7A41451F166D}" name="FK_User_Id" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{5BDF043D-B9D7-4535-B485-7A41451F166D}" name="FK_User_Id" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6440A10E-2A07-4DF1-9445-34115E04FFBD}" name="Tabelle4" displayName="Tabelle4" ref="I2:J5" totalsRowShown="0">
-  <autoFilter ref="I2:J5" xr:uid="{6440A10E-2A07-4DF1-9445-34115E04FFBD}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{627BBC57-220A-4739-92E2-F704A1342ACE}" name="Id"/>
-    <tableColumn id="2" xr3:uid="{601B9BF1-2C31-46A9-9129-0F00FE852AAE}" name="Enum_Value" dataDxfId="4"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1BCD61D6-66E0-4BCF-8CAA-424A30F8E612}" name="Tabelle5" displayName="Tabelle5" ref="A7:D10" totalsRowShown="0">
-  <autoFilter ref="A7:D10" xr:uid="{1BCD61D6-66E0-4BCF-8CAA-424A30F8E612}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1BCD61D6-66E0-4BCF-8CAA-424A30F8E612}" name="Tabelle5" displayName="Tabelle5" ref="I9:L12" totalsRowShown="0">
+  <autoFilter ref="I9:L12" xr:uid="{1BCD61D6-66E0-4BCF-8CAA-424A30F8E612}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8D4A3D16-6A52-406E-9540-500FC055E209}" name="Id"/>
     <tableColumn id="2" xr3:uid="{BA64696C-594D-4670-9C3C-502414C1963F}" name="Title"/>
@@ -308,21 +285,20 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{06B96A1C-9E52-4F51-BE49-D49282247183}" name="Tabelle6" displayName="Tabelle6" ref="I8:K11" totalsRowShown="0">
-  <autoFilter ref="I8:K11" xr:uid="{06B96A1C-9E52-4F51-BE49-D49282247183}"/>
-  <tableColumns count="3">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{06B96A1C-9E52-4F51-BE49-D49282247183}" name="Tabelle6" displayName="Tabelle6" ref="I2:J5" totalsRowShown="0">
+  <autoFilter ref="I2:J5" xr:uid="{06B96A1C-9E52-4F51-BE49-D49282247183}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C4A46AD2-D07A-43FF-A0A3-6CF7DF84E8CF}" name="Id"/>
     <tableColumn id="2" xr3:uid="{0D959709-F843-4301-8D2C-EC9669082C31}" name="Username"/>
-    <tableColumn id="3" xr3:uid="{2E54474C-F7CC-43E5-A1A5-7CA1DCFF5B67}" name="Spalte1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{229E6B1E-5B66-4257-BEBC-33B5012F86FA}" name="Tabelle8" displayName="Tabelle8" ref="A14:G15" totalsRowShown="0">
-  <autoFilter ref="A14:G15" xr:uid="{229E6B1E-5B66-4257-BEBC-33B5012F86FA}"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{229E6B1E-5B66-4257-BEBC-33B5012F86FA}" name="Tabelle8" displayName="Tabelle8" ref="A6:G7" totalsRowShown="0">
+  <autoFilter ref="A6:G7" xr:uid="{229E6B1E-5B66-4257-BEBC-33B5012F86FA}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9C09910E-FB02-449D-8784-3713F6BBC157}" name="Id"/>
     <tableColumn id="2" xr3:uid="{281E4E3A-6547-40C1-8BE0-9CA714117C26}" name="Username"/>
@@ -336,16 +312,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{53D21781-AEC9-4E4D-91A9-306B20FAB268}" name="Tabelle9" displayName="Tabelle9" ref="A19:F27" totalsRowShown="0">
-  <autoFilter ref="A19:F27" xr:uid="{53D21781-AEC9-4E4D-91A9-306B20FAB268}"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{53D21781-AEC9-4E4D-91A9-306B20FAB268}" name="Tabelle9" displayName="Tabelle9" ref="A12:F20" totalsRowShown="0">
+  <autoFilter ref="A12:F20" xr:uid="{53D21781-AEC9-4E4D-91A9-306B20FAB268}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E6392940-32AD-41C0-8D61-F093CA5840E8}" name="FK_Session_Id" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{A29A4273-E74B-40F2-965D-8D1C75A5D34F}" name="FK_Player_Id"/>
     <tableColumn id="3" xr3:uid="{7DC7DCAB-26DD-45D1-9D98-E713F6D01EB0}" name="FK_Game_Id"/>
     <tableColumn id="4" xr3:uid="{4AC58FAA-CFD1-46FC-ABD1-E218B78DD909}" name="DateOption"/>
     <tableColumn id="5" xr3:uid="{9B87213A-FA6C-447D-A45B-6B68131E7025}" name="FoodOption"/>
-    <tableColumn id="6" xr3:uid="{BA0CAA53-4FC1-45F5-9045-125414DEA338}" name="FK_Votevalue_Id"/>
+    <tableColumn id="6" xr3:uid="{BA0CAA53-4FC1-45F5-9045-125414DEA338}" name="Vote_value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -648,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A779D5AB-ACA6-4D62-9764-F021599A1A88}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,19 +641,18 @@
     <col min="7" max="7" width="13.88671875" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="21.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" customWidth="1"/>
-    <col min="12" max="12" width="15.21875" customWidth="1"/>
+    <col min="11" max="11" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -697,16 +672,16 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -732,197 +707,255 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45392</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
         <v>3</v>
       </c>
-      <c r="J5" t="s">
+      <c r="F15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="I8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>6</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="J10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I11">
-        <v>34</v>
-      </c>
-      <c r="J11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="1">
-        <v>45392</v>
-      </c>
-      <c r="F15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" t="s">
-        <v>46</v>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45347</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>14</v>
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45352</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>48</v>
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
-        <v>33</v>
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -932,124 +965,25 @@
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="F22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>45347</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>45352</v>
-      </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="E20" t="s">
         <v>18</v>
       </c>
-      <c r="F27">
-        <v>3</v>
+      <c r="F20" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C15" r:id="rId1" xr:uid="{A6E41F46-7F48-4801-B37B-5D2BC2494EC1}"/>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{A6E41F46-7F48-4801-B37B-5D2BC2494EC1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <tableParts count="6">
+  <tableParts count="5">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>